<commit_message>
mejorado smart pricing the stickers y ropa
</commit_message>
<xml_diff>
--- a/static/data/subcategories_complete-old-26122025.xlsx
+++ b/static/data/subcategories_complete-old-26122025.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="377">
   <si>
     <t>subcategory_slug</t>
   </si>
@@ -1133,9 +1133,6 @@
   </si>
   <si>
     <t>media/product_images/invitaciones_papeleria/tarjetas_de_menu/tarjetas-de-menu-detalle.jpg</t>
-  </si>
-  <si>
-    <t>media/product_images/packaging_alimentario/cajas_vasos_para_llevar/bolsas_para_llevar/bolsa-llevar.jpg</t>
   </si>
   <si>
     <t>media/product_images/ropa_y_bolsos/sombreros_pescador/atlantis-headwear-sustainable-bucket-ha_default.jpg</t>
@@ -1557,7 +1554,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -1583,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -1609,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -1635,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -1661,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -1687,7 +1684,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -1713,7 +1710,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -1739,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -1765,7 +1762,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -1791,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -1817,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -1843,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -1869,7 +1866,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -1895,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -1921,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -1947,7 +1944,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -1973,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -1999,7 +1996,7 @@
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -2025,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -2051,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H21" t="b">
         <v>1</v>
@@ -2077,7 +2074,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -2103,7 +2100,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H23" t="b">
         <v>0</v>
@@ -2129,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H24" t="b">
         <v>0</v>
@@ -2155,7 +2152,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H25" t="b">
         <v>0</v>
@@ -2181,7 +2178,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H26" t="b">
         <v>0</v>
@@ -2207,7 +2204,7 @@
         <v>0</v>
       </c>
       <c r="G27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H27" t="b">
         <v>1</v>
@@ -2233,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H28" t="b">
         <v>1</v>
@@ -2259,7 +2256,7 @@
         <v>0</v>
       </c>
       <c r="G29" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H29" t="b">
         <v>1</v>
@@ -2285,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H30" t="b">
         <v>1</v>
@@ -2311,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H31" t="b">
         <v>1</v>
@@ -2337,7 +2334,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H32" t="b">
         <v>0</v>
@@ -2363,7 +2360,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H33" t="b">
         <v>0</v>
@@ -2389,7 +2386,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H34" t="b">
         <v>0</v>
@@ -2415,7 +2412,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H35" t="b">
         <v>0</v>
@@ -2441,7 +2438,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H36" t="b">
         <v>1</v>
@@ -2467,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H37" t="b">
         <v>1</v>
@@ -2493,7 +2490,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H38" t="b">
         <v>1</v>
@@ -2519,7 +2516,7 @@
         <v>0</v>
       </c>
       <c r="G39" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H39" t="b">
         <v>1</v>
@@ -2545,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="G40" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H40" t="b">
         <v>1</v>
@@ -2571,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="G41" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H41" t="b">
         <v>1</v>
@@ -2597,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H42" t="b">
         <v>1</v>
@@ -2623,7 +2620,7 @@
         <v>0</v>
       </c>
       <c r="G43" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H43" t="b">
         <v>1</v>
@@ -2649,7 +2646,7 @@
         <v>0</v>
       </c>
       <c r="G44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H44" t="b">
         <v>1</v>
@@ -2675,7 +2672,7 @@
         <v>0</v>
       </c>
       <c r="G45" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H45" t="b">
         <v>1</v>
@@ -2701,7 +2698,7 @@
         <v>0</v>
       </c>
       <c r="G46" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H46" t="b">
         <v>1</v>
@@ -2727,7 +2724,7 @@
         <v>0</v>
       </c>
       <c r="G47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H47" t="b">
         <v>1</v>
@@ -2753,7 +2750,7 @@
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H48" t="b">
         <v>1</v>
@@ -2779,7 +2776,7 @@
         <v>0</v>
       </c>
       <c r="G49" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H49" t="b">
         <v>1</v>
@@ -2805,7 +2802,7 @@
         <v>0</v>
       </c>
       <c r="G50" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H50" t="b">
         <v>1</v>
@@ -2831,7 +2828,7 @@
         <v>0</v>
       </c>
       <c r="G51" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H51" t="b">
         <v>1</v>
@@ -2857,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H52" t="b">
         <v>1</v>
@@ -2883,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="G53" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H53" t="b">
         <v>1</v>
@@ -2909,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="G54" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H54" t="b">
         <v>0</v>
@@ -2935,7 +2932,7 @@
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H55" t="b">
         <v>0</v>
@@ -2961,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H56" t="b">
         <v>1</v>
@@ -2987,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="G57" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H57" t="b">
         <v>1</v>
@@ -3013,7 +3010,7 @@
         <v>0</v>
       </c>
       <c r="G58" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H58" t="b">
         <v>0</v>
@@ -3039,7 +3036,7 @@
         <v>0</v>
       </c>
       <c r="G59" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H59" t="b">
         <v>1</v>
@@ -3065,7 +3062,7 @@
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H60" t="b">
         <v>1</v>
@@ -3091,7 +3088,7 @@
         <v>0</v>
       </c>
       <c r="G61" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H61" t="b">
         <v>0</v>
@@ -3117,7 +3114,7 @@
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H62" t="b">
         <v>0</v>
@@ -3143,7 +3140,7 @@
         <v>0</v>
       </c>
       <c r="G63" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H63" t="b">
         <v>0</v>
@@ -3169,7 +3166,7 @@
         <v>0</v>
       </c>
       <c r="G64" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H64" t="b">
         <v>1</v>
@@ -3195,7 +3192,7 @@
         <v>0</v>
       </c>
       <c r="G65" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H65" t="b">
         <v>1</v>
@@ -3221,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H66" t="b">
         <v>1</v>
@@ -3247,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="G67" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H67" t="b">
         <v>0</v>
@@ -3273,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H68" t="b">
         <v>0</v>
@@ -3299,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H69" t="b">
         <v>0</v>
@@ -3325,7 +3322,7 @@
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H70" t="b">
         <v>1</v>
@@ -3351,7 +3348,7 @@
         <v>0</v>
       </c>
       <c r="G71" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
@@ -3377,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H72" t="b">
         <v>0</v>
@@ -3403,7 +3400,7 @@
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H73" t="b">
         <v>1</v>
@@ -3429,7 +3426,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H74" t="b">
         <v>0</v>
@@ -3455,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="G75" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H75" t="b">
         <v>0</v>
@@ -3481,7 +3478,7 @@
         <v>0</v>
       </c>
       <c r="G76" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H76" t="b">
         <v>1</v>
@@ -3507,7 +3504,7 @@
         <v>0</v>
       </c>
       <c r="G77" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H77" t="b">
         <v>0</v>
@@ -3533,7 +3530,7 @@
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H78" t="b">
         <v>0</v>
@@ -3559,7 +3556,7 @@
         <v>0</v>
       </c>
       <c r="G79" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H79" t="b">
         <v>0</v>
@@ -3585,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="G80" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H80" t="b">
         <v>1</v>
@@ -3611,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H81" t="b">
         <v>1</v>
@@ -3637,7 +3634,7 @@
         <v>0</v>
       </c>
       <c r="G82" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H82" t="b">
         <v>1</v>
@@ -3663,7 +3660,7 @@
         <v>0</v>
       </c>
       <c r="G83" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H83" t="b">
         <v>1</v>
@@ -3689,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H84" t="b">
         <v>1</v>
@@ -3715,7 +3712,7 @@
         <v>0</v>
       </c>
       <c r="G85" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H85" t="b">
         <v>1</v>
@@ -3741,7 +3738,7 @@
         <v>0</v>
       </c>
       <c r="G86" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H86" t="b">
         <v>1</v>
@@ -3767,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="G87" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H87" t="b">
         <v>1</v>
@@ -3793,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H88" t="b">
         <v>1</v>
@@ -3812,14 +3809,11 @@
       <c r="D89" t="s">
         <v>282</v>
       </c>
-      <c r="E89" t="s">
-        <v>373</v>
-      </c>
       <c r="F89">
         <v>0</v>
       </c>
       <c r="G89" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H89" t="b">
         <v>1</v>
@@ -3839,13 +3833,13 @@
         <v>283</v>
       </c>
       <c r="E90" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F90">
         <v>0</v>
       </c>
       <c r="G90" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H90" t="b">
         <v>1</v>
@@ -3865,13 +3859,13 @@
         <v>284</v>
       </c>
       <c r="E91" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F91">
         <v>0</v>
       </c>
       <c r="G91" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H91" t="b">
         <v>1</v>
@@ -3894,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H92" t="b">
         <v>1</v>

</xml_diff>